<commit_message>
augmenting heat pump analysis pipeline and visualization of results
</commit_message>
<xml_diff>
--- a/retrofit_costs/tare_retrofit_costs_cpi.xlsx
+++ b/retrofit_costs/tare_retrofit_costs_cpi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14128\Research\cmu-tare-model\retrofit_costs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnav\Documents\Research\Trane_Technologies\cmu-tare-model\retrofit_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0125ABC6-9D58-4437-B9C9-C81A1A5E2770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD343C19-D05D-4E82-A74B-F311F617230D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="738" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="738" activeTab="1" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
   </bookViews>
   <sheets>
     <sheet name="cpi" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="133">
   <si>
     <t>$/unit</t>
   </si>
@@ -425,6 +425,21 @@
   </si>
   <si>
     <t>cpi_ratio</t>
+  </si>
+  <si>
+    <t>Electric ASHP - Ducted</t>
+  </si>
+  <si>
+    <t>Data Year 2025</t>
+  </si>
+  <si>
+    <t>SEER 15, 8.8 HSPF</t>
+  </si>
+  <si>
+    <t>SEER 16, 8.8 HSPF</t>
+  </si>
+  <si>
+    <t>Trane</t>
   </si>
 </sst>
 </file>
@@ -432,7 +447,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#0.000"/>
+    <numFmt numFmtId="164" formatCode="#0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -541,7 +556,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -867,11 +882,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3734CD01-6A61-4B41-8376-4D55F8F15FCB}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>125</v>
       </c>
@@ -879,7 +894,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>2010</v>
       </c>
@@ -887,7 +902,7 @@
         <v>218.05600000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>2011</v>
       </c>
@@ -895,7 +910,7 @@
         <v>224.93899999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>2012</v>
       </c>
@@ -903,7 +918,7 @@
         <v>229.59399999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>2013</v>
       </c>
@@ -911,7 +926,7 @@
         <v>232.95699999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>2014</v>
       </c>
@@ -919,7 +934,7 @@
         <v>236.73599999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>2015</v>
       </c>
@@ -927,7 +942,7 @@
         <v>237.017</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>2016</v>
       </c>
@@ -935,7 +950,7 @@
         <v>240.00700000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>2017</v>
       </c>
@@ -943,7 +958,7 @@
         <v>245.12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>2018</v>
       </c>
@@ -951,7 +966,7 @@
         <v>251.107</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>2019</v>
       </c>
@@ -959,7 +974,7 @@
         <v>255.65700000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>2020</v>
       </c>
@@ -967,7 +982,7 @@
         <v>258.81099999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>2021</v>
       </c>
@@ -975,7 +990,7 @@
         <v>270.97000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>2022</v>
       </c>
@@ -983,7 +998,7 @@
         <v>292.65499999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>2023</v>
       </c>
@@ -998,34 +1013,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25BD77E-F6CE-47DE-940C-0B686D6456B3}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="24.5546875" customWidth="1"/>
-    <col min="12" max="12" width="23.21875" customWidth="1"/>
-    <col min="13" max="13" width="26.21875" customWidth="1"/>
-    <col min="14" max="14" width="20.77734375" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" customWidth="1"/>
-    <col min="16" max="16" width="23.5546875" customWidth="1"/>
-    <col min="19" max="19" width="38.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="9" max="9" width="17.90625" customWidth="1"/>
+    <col min="10" max="10" width="19.6328125" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" customWidth="1"/>
+    <col min="12" max="12" width="23.1796875" customWidth="1"/>
+    <col min="13" max="13" width="26.1796875" customWidth="1"/>
+    <col min="14" max="14" width="20.81640625" customWidth="1"/>
+    <col min="15" max="15" width="17.81640625" customWidth="1"/>
+    <col min="16" max="16" width="23.54296875" customWidth="1"/>
+    <col min="19" max="19" width="38.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1084,7 +1099,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1144,7 +1159,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -1204,7 +1219,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -1264,7 +1279,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1324,7 +1339,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1374,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="10">
-        <f t="shared" ref="P6:P9" si="2">$O6+($O6-$N6)</f>
+        <f t="shared" ref="P6:P11" si="2">$O6+($O6-$N6)</f>
         <v>0</v>
       </c>
       <c r="Q6">
@@ -1387,7 +1402,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1450,7 +1465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1513,7 +1528,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1574,6 +1589,126 @@
       </c>
       <c r="S9" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10">
+        <v>2025</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>6654.7500000000018</v>
+      </c>
+      <c r="I10">
+        <v>8151.0350000000008</v>
+      </c>
+      <c r="J10">
+        <v>9647.32</v>
+      </c>
+      <c r="K10">
+        <v>87.852499999999964</v>
+      </c>
+      <c r="L10">
+        <v>95.945416666666631</v>
+      </c>
+      <c r="M10">
+        <v>104.03833333333331</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="8">
+        <v>0</v>
+      </c>
+      <c r="P10" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>25</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11">
+        <v>2025</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>7864.9399999999987</v>
+      </c>
+      <c r="I11">
+        <v>8664.32</v>
+      </c>
+      <c r="J11">
+        <v>9463.6999999999989</v>
+      </c>
+      <c r="K11">
+        <v>93.546666666666681</v>
+      </c>
+      <c r="L11">
+        <v>102.6179166666667</v>
+      </c>
+      <c r="M11">
+        <v>111.68916666666671</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="8">
+        <v>0</v>
+      </c>
+      <c r="P11" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>25</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1595,24 +1730,24 @@
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="25.109375" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.90625" customWidth="1"/>
+    <col min="9" max="9" width="19.54296875" customWidth="1"/>
+    <col min="10" max="10" width="19.6328125" customWidth="1"/>
+    <col min="11" max="11" width="25.08984375" customWidth="1"/>
+    <col min="12" max="12" width="23.36328125" customWidth="1"/>
     <col min="13" max="13" width="25" customWidth="1"/>
-    <col min="14" max="15" width="10.5546875" customWidth="1"/>
-    <col min="16" max="16" width="40.44140625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="10.54296875" customWidth="1"/>
+    <col min="16" max="16" width="40.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1666,7 +1801,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1717,7 +1852,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -1768,7 +1903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -1819,7 +1954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1870,7 +2005,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -1921,7 +2056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1973,7 +2108,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -2025,7 +2160,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -2077,7 +2212,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -2086,7 +2221,7 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -2095,7 +2230,7 @@
       <c r="F11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -2104,7 +2239,7 @@
       <c r="F12"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -2113,7 +2248,7 @@
       <c r="F13"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -2122,7 +2257,7 @@
       <c r="F14"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -2131,7 +2266,7 @@
       <c r="F15"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -2140,7 +2275,7 @@
       <c r="F16"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -2149,7 +2284,7 @@
       <c r="F17"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -2158,7 +2293,7 @@
       <c r="F18"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -2167,7 +2302,7 @@
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -2176,7 +2311,7 @@
       <c r="F20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -2185,7 +2320,7 @@
       <c r="F21"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -2194,7 +2329,7 @@
       <c r="F22"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -2203,7 +2338,7 @@
       <c r="F23"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -2212,7 +2347,7 @@
       <c r="F24"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -2221,7 +2356,7 @@
       <c r="F25"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -2230,7 +2365,7 @@
       <c r="F26"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -2239,7 +2374,7 @@
       <c r="F27"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -2248,7 +2383,7 @@
       <c r="F28"/>
       <c r="G28"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -2257,7 +2392,7 @@
       <c r="F29"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -2266,7 +2401,7 @@
       <c r="F30"/>
       <c r="G30"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -2275,7 +2410,7 @@
       <c r="F31"/>
       <c r="G31"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -2284,7 +2419,7 @@
       <c r="F32"/>
       <c r="G32"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -2293,7 +2428,7 @@
       <c r="F33"/>
       <c r="G33"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
@@ -2302,7 +2437,7 @@
       <c r="F34"/>
       <c r="G34"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -2311,7 +2446,7 @@
       <c r="F35"/>
       <c r="G35"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
@@ -2320,7 +2455,7 @@
       <c r="F36"/>
       <c r="G36"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -2329,7 +2464,7 @@
       <c r="F37"/>
       <c r="G37"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -2338,7 +2473,7 @@
       <c r="F38"/>
       <c r="G38"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -2347,7 +2482,7 @@
       <c r="F39"/>
       <c r="G39"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -2356,7 +2491,7 @@
       <c r="F40"/>
       <c r="G40"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -2365,7 +2500,7 @@
       <c r="F41"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -2374,7 +2509,7 @@
       <c r="F42"/>
       <c r="G42"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -2383,7 +2518,7 @@
       <c r="F43"/>
       <c r="G43"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -2392,7 +2527,7 @@
       <c r="F44"/>
       <c r="G44"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -2401,7 +2536,7 @@
       <c r="F45"/>
       <c r="G45"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -2410,7 +2545,7 @@
       <c r="F46"/>
       <c r="G46"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -2419,7 +2554,7 @@
       <c r="F47"/>
       <c r="G47"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -2428,7 +2563,7 @@
       <c r="F48"/>
       <c r="G48"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -2437,7 +2572,7 @@
       <c r="F49"/>
       <c r="G49"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
@@ -2446,7 +2581,7 @@
       <c r="F50"/>
       <c r="G50"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -2455,7 +2590,7 @@
       <c r="F51"/>
       <c r="G51"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -2464,7 +2599,7 @@
       <c r="F52"/>
       <c r="G52"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -2473,7 +2608,7 @@
       <c r="F53"/>
       <c r="G53"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -2482,7 +2617,7 @@
       <c r="F54"/>
       <c r="G54"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -2491,7 +2626,7 @@
       <c r="F55"/>
       <c r="G55"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
@@ -2500,7 +2635,7 @@
       <c r="F56"/>
       <c r="G56"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
@@ -2509,7 +2644,7 @@
       <c r="F57"/>
       <c r="G57"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -2518,7 +2653,7 @@
       <c r="F58"/>
       <c r="G58"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -2527,7 +2662,7 @@
       <c r="F59"/>
       <c r="G59"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -2536,7 +2671,7 @@
       <c r="F60"/>
       <c r="G60"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -2545,7 +2680,7 @@
       <c r="F61"/>
       <c r="G61"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -2554,7 +2689,7 @@
       <c r="F62"/>
       <c r="G62"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -2563,7 +2698,7 @@
       <c r="F63"/>
       <c r="G63"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
@@ -2572,7 +2707,7 @@
       <c r="F64"/>
       <c r="G64"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
@@ -2581,7 +2716,7 @@
       <c r="F65"/>
       <c r="G65"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
@@ -2590,7 +2725,7 @@
       <c r="F66"/>
       <c r="G66"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
@@ -2599,7 +2734,7 @@
       <c r="F67"/>
       <c r="G67"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
@@ -2608,7 +2743,7 @@
       <c r="F68"/>
       <c r="G68"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
@@ -2617,7 +2752,7 @@
       <c r="F69"/>
       <c r="G69"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
@@ -2626,7 +2761,7 @@
       <c r="F70"/>
       <c r="G70"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -2635,7 +2770,7 @@
       <c r="F71"/>
       <c r="G71"/>
     </row>
-    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
@@ -2646,7 +2781,7 @@
       <c r="N72"/>
       <c r="O72"/>
     </row>
-    <row r="73" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
@@ -2657,7 +2792,7 @@
       <c r="N73"/>
       <c r="O73"/>
     </row>
-    <row r="74" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
@@ -2668,7 +2803,7 @@
       <c r="N74"/>
       <c r="O74"/>
     </row>
-    <row r="75" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
@@ -2679,7 +2814,7 @@
       <c r="N75"/>
       <c r="O75"/>
     </row>
-    <row r="76" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
@@ -2690,7 +2825,7 @@
       <c r="N76"/>
       <c r="O76"/>
     </row>
-    <row r="77" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
@@ -2701,7 +2836,7 @@
       <c r="N77"/>
       <c r="O77"/>
     </row>
-    <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
@@ -2712,7 +2847,7 @@
       <c r="N78"/>
       <c r="O78"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
@@ -2721,7 +2856,7 @@
       <c r="F79"/>
       <c r="G79"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
@@ -2730,7 +2865,7 @@
       <c r="F80"/>
       <c r="G80"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
@@ -2739,7 +2874,7 @@
       <c r="F81"/>
       <c r="G81"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
@@ -2748,7 +2883,7 @@
       <c r="F82"/>
       <c r="G82"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
@@ -2757,7 +2892,7 @@
       <c r="F83"/>
       <c r="G83"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
@@ -2766,7 +2901,7 @@
       <c r="F84"/>
       <c r="G84"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
@@ -2775,7 +2910,7 @@
       <c r="F85"/>
       <c r="G85"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
@@ -2784,7 +2919,7 @@
       <c r="F86"/>
       <c r="G86"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
@@ -2793,7 +2928,7 @@
       <c r="F87"/>
       <c r="G87"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
@@ -2802,7 +2937,7 @@
       <c r="F88"/>
       <c r="G88"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
@@ -2811,7 +2946,7 @@
       <c r="F89"/>
       <c r="G89"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
@@ -2820,7 +2955,7 @@
       <c r="F90"/>
       <c r="G90"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
@@ -2829,7 +2964,7 @@
       <c r="F91"/>
       <c r="G91"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -2838,7 +2973,7 @@
       <c r="F92"/>
       <c r="G92"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
@@ -2847,7 +2982,7 @@
       <c r="F93"/>
       <c r="G93"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
@@ -2856,7 +2991,7 @@
       <c r="F94"/>
       <c r="G94"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95"/>
@@ -2881,21 +3016,21 @@
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="11.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
-    <col min="8" max="8" width="19.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" customWidth="1"/>
-    <col min="14" max="14" width="39.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="11.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" customWidth="1"/>
+    <col min="6" max="6" width="11.6328125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.08984375" customWidth="1"/>
+    <col min="11" max="11" width="11.08984375" customWidth="1"/>
+    <col min="14" max="14" width="39.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2939,7 +3074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -2984,7 +3119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -3029,7 +3164,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -3074,7 +3209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -3120,7 +3255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -3165,475 +3300,475 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97"/>
       <c r="B97"/>
       <c r="C97"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98"/>
       <c r="B98"/>
       <c r="C98"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
@@ -3653,21 +3788,21 @@
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="9" width="19.109375" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" customWidth="1"/>
-    <col min="14" max="14" width="41.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="8" max="9" width="19.08984375" customWidth="1"/>
+    <col min="10" max="10" width="20.08984375" customWidth="1"/>
+    <col min="11" max="11" width="11.36328125" customWidth="1"/>
+    <col min="14" max="14" width="41.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -3711,7 +3846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -3756,7 +3891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -3801,7 +3936,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -3846,7 +3981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -3892,7 +4027,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -3938,11 +4073,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7"/>
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
@@ -3957,381 +4092,381 @@
       <c r="L8" s="2"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9"/>
       <c r="C9"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10"/>
       <c r="C10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11"/>
       <c r="C11"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14"/>
       <c r="C14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15"/>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16"/>
       <c r="C16"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17"/>
       <c r="C17"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18"/>
       <c r="C18"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19"/>
       <c r="C19"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20"/>
       <c r="C20"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="C21"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22"/>
       <c r="C22"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23"/>
       <c r="C23"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24"/>
       <c r="C24"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25"/>
       <c r="C25"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26"/>
       <c r="C26"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27"/>
       <c r="C27"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28"/>
       <c r="C28"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29"/>
       <c r="C29"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30"/>
       <c r="C30"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31"/>
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32"/>
       <c r="C32"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33"/>
       <c r="C33"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34"/>
       <c r="C34"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35"/>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36"/>
       <c r="C36"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37"/>
       <c r="C37"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38"/>
       <c r="C38"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39"/>
       <c r="C39"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40"/>
       <c r="C40"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41"/>
       <c r="C41"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42"/>
       <c r="C42"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43"/>
       <c r="C43"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44"/>
       <c r="C44"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45"/>
       <c r="C45"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46"/>
       <c r="C46"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47"/>
       <c r="C47"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48"/>
       <c r="C48"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49"/>
       <c r="C49"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50"/>
       <c r="C50"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51"/>
       <c r="C51"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52"/>
       <c r="C52"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53"/>
       <c r="C53"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54"/>
       <c r="C54"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55"/>
       <c r="C55"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56"/>
       <c r="C56"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57"/>
       <c r="C57"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58"/>
       <c r="C58"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59"/>
       <c r="C59"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60"/>
       <c r="C60"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61"/>
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62"/>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63"/>
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64"/>
       <c r="C64"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65"/>
       <c r="C65"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66"/>
       <c r="C66"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67"/>
       <c r="C67"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68"/>
       <c r="C68"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69"/>
       <c r="C69"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70"/>
       <c r="C70"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71"/>
       <c r="C71"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72"/>
       <c r="C72"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73"/>
       <c r="C73"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74"/>
       <c r="C74"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75"/>
       <c r="C75"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76"/>
       <c r="C76"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77"/>
       <c r="C77"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78"/>
       <c r="C78"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79"/>
       <c r="C79"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80"/>
       <c r="C80"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81"/>
       <c r="C81"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82"/>
       <c r="C82"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83"/>
       <c r="C83"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84"/>
       <c r="C84"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85"/>
       <c r="C85"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86"/>
       <c r="C86"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87"/>
       <c r="C87"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88"/>
       <c r="C88"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89"/>
       <c r="C89"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90"/>
       <c r="C90"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91"/>
       <c r="C91"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92"/>
       <c r="C92"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93"/>
       <c r="C93"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94"/>
       <c r="C94"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95"/>
       <c r="C95"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96"/>
       <c r="C96"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97"/>
       <c r="C97"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98"/>
       <c r="C98"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99"/>
       <c r="C99"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100"/>
       <c r="C100"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101"/>
       <c r="C101"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102"/>
       <c r="C102"/>
     </row>
@@ -4351,19 +4486,19 @@
       <selection pane="topRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="4" max="5" width="23.6640625" customWidth="1"/>
-    <col min="6" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="10" width="25.5546875" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" customWidth="1"/>
-    <col min="12" max="12" width="51.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" customWidth="1"/>
+    <col min="4" max="5" width="23.6328125" customWidth="1"/>
+    <col min="6" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="10" width="25.54296875" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" customWidth="1"/>
+    <col min="12" max="12" width="51.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4401,7 +4536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>73</v>
       </c>
@@ -4441,7 +4576,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>73</v>
       </c>
@@ -4481,7 +4616,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>73</v>
       </c>
@@ -4521,7 +4656,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>73</v>
       </c>
@@ -4561,7 +4696,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>73</v>
       </c>
@@ -4601,7 +4736,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>73</v>
       </c>
@@ -4641,7 +4776,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>73</v>
       </c>
@@ -4681,7 +4816,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>73</v>
       </c>
@@ -4721,7 +4856,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>73</v>
       </c>
@@ -4761,7 +4896,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>73</v>
       </c>
@@ -4801,7 +4936,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>73</v>
       </c>
@@ -4841,7 +4976,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>73</v>
       </c>
@@ -4881,7 +5016,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>73</v>
       </c>
@@ -4921,7 +5056,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>73</v>
       </c>
@@ -4961,7 +5096,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>73</v>
       </c>
@@ -5001,7 +5136,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>73</v>
       </c>
@@ -5041,7 +5176,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>73</v>
       </c>
@@ -5081,7 +5216,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>73</v>
       </c>
@@ -5121,7 +5256,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>73</v>
       </c>
@@ -5161,7 +5296,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>104</v>
       </c>
@@ -5201,7 +5336,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>104</v>
       </c>
@@ -5241,7 +5376,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>104</v>
       </c>
@@ -5281,7 +5416,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
created new TARE output CSVs after fixing cooling equipment consideration
</commit_message>
<xml_diff>
--- a/retrofit_costs/tare_retrofit_costs_cpi.xlsx
+++ b/retrofit_costs/tare_retrofit_costs_cpi.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnav\Documents\Research\Trane_Technologies\cmu-tare-model\retrofit_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD343C19-D05D-4E82-A74B-F311F617230D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BAD53B-B10D-4D03-8287-33E4ACE6CF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="738" activeTab="1" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="738" firstSheet="1" activeTab="1" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
   </bookViews>
   <sheets>
     <sheet name="cpi" sheetId="7" r:id="rId1"/>
     <sheet name="heating_costs" sheetId="1" r:id="rId2"/>
-    <sheet name="waterHeating_costs" sheetId="3" r:id="rId3"/>
-    <sheet name="clothesDrying_costs" sheetId="4" r:id="rId4"/>
-    <sheet name="cooking_costs" sheetId="5" r:id="rId5"/>
-    <sheet name="enclosure_upgrade_costs" sheetId="6" r:id="rId6"/>
+    <sheet name="cooling_costs" sheetId="8" r:id="rId3"/>
+    <sheet name="waterHeating_costs" sheetId="3" r:id="rId4"/>
+    <sheet name="clothesDrying_costs" sheetId="4" r:id="rId5"/>
+    <sheet name="cooking_costs" sheetId="5" r:id="rId6"/>
+    <sheet name="enclosure_upgrade_costs" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="140">
   <si>
     <t>$/unit</t>
   </si>
@@ -440,6 +441,27 @@
   </si>
   <si>
     <t>Trane</t>
+  </si>
+  <si>
+    <t>Central AC</t>
+  </si>
+  <si>
+    <t>Room AC</t>
+  </si>
+  <si>
+    <t>SEER 15</t>
+  </si>
+  <si>
+    <t>EER 12</t>
+  </si>
+  <si>
+    <t>Data Year 2025.</t>
+  </si>
+  <si>
+    <t>Data Year 2025. Zeroed since the same equipment is accounted for in heating costs</t>
+  </si>
+  <si>
+    <t>OLD Numbers for Electric ASHP</t>
   </si>
 </sst>
 </file>
@@ -1013,11 +1035,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25BD77E-F6CE-47DE-940C-0B686D6456B3}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1344,7 +1366,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -1389,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="10">
-        <f t="shared" ref="P6:P11" si="2">$O6+($O6-$N6)</f>
+        <f t="shared" ref="P6:P12" si="2">$O6+($O6-$N6)</f>
         <v>0</v>
       </c>
       <c r="Q6">
@@ -1709,6 +1731,66 @@
       </c>
       <c r="S11" s="1" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>2025</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0</v>
+      </c>
+      <c r="P12" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>15</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1722,6 +1804,398 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C73B86-AA0C-4F9D-B521-F691E24A6513}">
+  <dimension ref="A1:S6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="9" max="9" width="17.90625" customWidth="1"/>
+    <col min="10" max="10" width="19.6328125" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" customWidth="1"/>
+    <col min="12" max="12" width="23.1796875" customWidth="1"/>
+    <col min="13" max="13" width="26.1796875" customWidth="1"/>
+    <col min="14" max="14" width="20.81640625" customWidth="1"/>
+    <col min="15" max="15" width="17.81640625" customWidth="1"/>
+    <col min="16" max="16" width="23.54296875" customWidth="1"/>
+    <col min="19" max="19" width="38.36328125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2">
+        <v>2025</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2728.97</v>
+      </c>
+      <c r="I2" s="8">
+        <v>4548.26</v>
+      </c>
+      <c r="J2" s="10">
+        <v>6367.55</v>
+      </c>
+      <c r="K2" s="5">
+        <v>227.41416666666666</v>
+      </c>
+      <c r="L2" s="8">
+        <v>379.0216666666667</v>
+      </c>
+      <c r="M2" s="10">
+        <v>530.62916666666672</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0</v>
+      </c>
+      <c r="O2" s="8">
+        <v>0</v>
+      </c>
+      <c r="P2" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>25</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3">
+        <v>2025</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
+        <v>377.79000000000019</v>
+      </c>
+      <c r="I3" s="8">
+        <v>438.7199999999998</v>
+      </c>
+      <c r="J3" s="10">
+        <v>660.34999999999991</v>
+      </c>
+      <c r="K3" s="5">
+        <v>31.482500000000016</v>
+      </c>
+      <c r="L3" s="8">
+        <v>36.559999999999981</v>
+      </c>
+      <c r="M3" s="10">
+        <v>55.029166666666661</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="8">
+        <v>0</v>
+      </c>
+      <c r="P3" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>25</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2025</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
+        <v>6188.8900000000021</v>
+      </c>
+      <c r="I4" s="8">
+        <v>11237.48</v>
+      </c>
+      <c r="J4" s="10">
+        <v>16286.07</v>
+      </c>
+      <c r="K4" s="5">
+        <v>515.74083333333351</v>
+      </c>
+      <c r="L4" s="8">
+        <v>936.45666666666659</v>
+      </c>
+      <c r="M4" s="10">
+        <v>1357.1724999999999</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="8">
+        <v>0</v>
+      </c>
+      <c r="P4" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>25</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5">
+        <v>2025</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0</v>
+      </c>
+      <c r="P5" s="10">
+        <f t="shared" ref="P5:P6" si="0">$O5+($O5-$N5)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>25</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6">
+        <v>2025</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="8">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>25</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FBB1F9-AA0F-4F3E-92E1-FA5D825DBAEF}">
   <dimension ref="A1:T95"/>
   <sheetViews>
@@ -3007,7 +3481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51DF997B-B96C-4908-A8E2-238F90744569}">
   <dimension ref="A1:N101"/>
   <sheetViews>
@@ -3779,7 +4253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4F662D-1BD7-4400-95A3-A4A7CEFF8447}">
   <dimension ref="A1:N102"/>
   <sheetViews>
@@ -4477,7 +4951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AAB083-F7AB-4F7C-A5E9-54BE3CB88F43}">
   <dimension ref="A1:L24"/>
   <sheetViews>

</xml_diff>

<commit_message>
misc changes to figures, prior to beginning sensitivity analyses
</commit_message>
<xml_diff>
--- a/retrofit_costs/tare_retrofit_costs_cpi.xlsx
+++ b/retrofit_costs/tare_retrofit_costs_cpi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnav\Documents\Research\Trane_Technologies\cmu-tare-model\retrofit_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BAD53B-B10D-4D03-8287-33E4ACE6CF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA9E09A-1D9F-42C6-8B2A-6360FB60EBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="738" firstSheet="1" activeTab="1" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="738" firstSheet="1" activeTab="2" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
   </bookViews>
   <sheets>
     <sheet name="cpi" sheetId="7" r:id="rId1"/>
@@ -1037,9 +1037,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25BD77E-F6CE-47DE-940C-0B686D6456B3}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1807,9 +1807,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C73B86-AA0C-4F9D-B521-F691E24A6513}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
new run with trane technologies replacement costs
</commit_message>
<xml_diff>
--- a/retrofit_costs/tare_retrofit_costs_cpi.xlsx
+++ b/retrofit_costs/tare_retrofit_costs_cpi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnav\Documents\Research\Trane_Technologies\cmu-tare-model\retrofit_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA9E09A-1D9F-42C6-8B2A-6360FB60EBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF23C1C4-9ABF-4CF4-B1B7-C133CB20563F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="738" firstSheet="1" activeTab="2" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="738" firstSheet="1" activeTab="1" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
   </bookViews>
   <sheets>
     <sheet name="cpi" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="143">
   <si>
     <t>$/unit</t>
   </si>
@@ -462,6 +462,15 @@
   </si>
   <si>
     <t>OLD Numbers for Electric ASHP</t>
+  </si>
+  <si>
+    <t>Trane Central AC</t>
+  </si>
+  <si>
+    <t>Trane Natural Gas and Propane Furnace</t>
+  </si>
+  <si>
+    <t>96 AFUE</t>
   </si>
 </sst>
 </file>
@@ -1035,11 +1044,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25BD77E-F6CE-47DE-940C-0B686D6456B3}">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1186,41 +1195,40 @@
         <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="E3">
-        <v>2013</v>
+        <v>2025</v>
       </c>
       <c r="F3">
-        <f>cpi!$B$15/cpi!$B$5</f>
-        <v>1.3079752915774157</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" s="5">
-        <v>1600</v>
+        <v>3292.5600000000004</v>
       </c>
       <c r="I3" s="8">
-        <v>1600</v>
+        <v>3421.92</v>
       </c>
       <c r="J3" s="10">
-        <v>1600</v>
+        <v>3551.2799999999997</v>
       </c>
       <c r="K3" s="5">
-        <v>50</v>
+        <v>7.8539999999999965</v>
       </c>
       <c r="L3" s="8">
-        <v>50</v>
+        <v>8.5470000000000024</v>
       </c>
       <c r="M3" s="10">
-        <v>50</v>
+        <v>9.2400000000000091</v>
       </c>
       <c r="N3" s="5">
         <v>0</v>
@@ -1235,10 +1243,10 @@
         <v>20</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
@@ -1246,13 +1254,13 @@
         <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>2013</v>
@@ -1265,22 +1273,22 @@
         <v>1</v>
       </c>
       <c r="H4" s="5">
-        <v>4100</v>
+        <v>1600</v>
       </c>
       <c r="I4" s="8">
-        <v>4100</v>
+        <v>1600</v>
       </c>
       <c r="J4" s="10">
-        <v>4100</v>
+        <v>1600</v>
       </c>
       <c r="K4" s="5">
-        <v>3.9</v>
+        <v>50</v>
       </c>
       <c r="L4" s="8">
-        <v>3.9</v>
+        <v>50</v>
       </c>
       <c r="M4" s="10">
-        <v>3.9</v>
+        <v>50</v>
       </c>
       <c r="N4" s="5">
         <v>0</v>
@@ -1292,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>11</v>
@@ -1306,13 +1314,13 @@
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>2013</v>
@@ -1325,13 +1333,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="5">
-        <v>3800</v>
+        <v>4100</v>
       </c>
       <c r="I5" s="8">
-        <v>3800</v>
+        <v>4100</v>
       </c>
       <c r="J5" s="10">
-        <v>3800</v>
+        <v>4100</v>
       </c>
       <c r="K5" s="5">
         <v>3.9</v>
@@ -1352,7 +1360,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>11</v>
@@ -1361,18 +1369,18 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>139</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
       </c>
       <c r="E6">
         <v>2013</v>
@@ -1385,24 +1393,22 @@
         <v>1</v>
       </c>
       <c r="H6" s="5">
-        <v>3700</v>
+        <v>3800</v>
       </c>
       <c r="I6" s="8">
-        <v>4800</v>
+        <v>3800</v>
       </c>
       <c r="J6" s="10">
-        <f t="shared" ref="J6:J9" si="0">$I6+($I6-$H6)</f>
-        <v>5900</v>
+        <v>3800</v>
       </c>
       <c r="K6" s="5">
-        <v>42</v>
+        <v>3.9</v>
       </c>
       <c r="L6" s="8">
-        <v>55</v>
+        <v>3.9</v>
       </c>
       <c r="M6" s="10">
-        <f t="shared" ref="M6:M9" si="1">$L6+($L6-$K6)</f>
-        <v>68</v>
+        <v>3.9</v>
       </c>
       <c r="N6" s="5">
         <v>0</v>
@@ -1411,17 +1417,16 @@
         <v>0</v>
       </c>
       <c r="P6" s="10">
-        <f t="shared" ref="P6:P12" si="2">$O6+($O6-$N6)</f>
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="29" x14ac:dyDescent="0.35">
@@ -1429,13 +1434,13 @@
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>139</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>2013</v>
@@ -1448,34 +1453,34 @@
         <v>1</v>
       </c>
       <c r="H7" s="5">
-        <v>1800</v>
+        <v>3700</v>
       </c>
       <c r="I7" s="8">
-        <v>2300</v>
+        <v>4800</v>
       </c>
       <c r="J7" s="10">
-        <f t="shared" si="0"/>
-        <v>2800</v>
+        <f t="shared" ref="J7:J10" si="0">$I7+($I7-$H7)</f>
+        <v>5900</v>
       </c>
       <c r="K7" s="5">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="L7" s="8">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="M7" s="10">
-        <f t="shared" si="1"/>
-        <v>105</v>
+        <f t="shared" ref="M7:M10" si="1">$L7+($L7-$K7)</f>
+        <v>68</v>
       </c>
       <c r="N7" s="5">
-        <v>490</v>
+        <v>0</v>
       </c>
       <c r="O7" s="8">
-        <v>630</v>
+        <v>0</v>
       </c>
       <c r="P7" s="10">
-        <f t="shared" si="2"/>
-        <v>770</v>
+        <f t="shared" ref="P7:P13" si="2">$O7+($O7-$N7)</f>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>15</v>
@@ -1487,18 +1492,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E8">
         <v>2013</v>
@@ -1508,37 +1513,37 @@
         <v>1.3079752915774157</v>
       </c>
       <c r="G8">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="H8" s="5">
-        <v>2340</v>
+        <v>1800</v>
       </c>
       <c r="I8" s="8">
-        <v>2990</v>
+        <v>2300</v>
       </c>
       <c r="J8" s="10">
         <f t="shared" si="0"/>
-        <v>3640</v>
+        <v>2800</v>
       </c>
       <c r="K8" s="5">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="L8" s="8">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="M8" s="10">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="N8" s="5">
-        <v>1690</v>
+        <v>490</v>
       </c>
       <c r="O8" s="8">
-        <v>2210</v>
+        <v>630</v>
       </c>
       <c r="P8" s="10">
         <f t="shared" si="2"/>
-        <v>2730</v>
+        <v>770</v>
       </c>
       <c r="Q8">
         <v>15</v>
@@ -1547,7 +1552,7 @@
         <v>11</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
@@ -1555,13 +1560,13 @@
         <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E9">
         <v>2013</v>
@@ -1571,37 +1576,37 @@
         <v>1.3079752915774157</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="H9" s="5">
-        <v>1800</v>
+        <v>2340</v>
       </c>
       <c r="I9" s="8">
-        <v>2300</v>
+        <v>2990</v>
       </c>
       <c r="J9" s="10">
         <f t="shared" si="0"/>
-        <v>2800</v>
+        <v>3640</v>
       </c>
       <c r="K9" s="5">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="L9" s="8">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="M9" s="10">
         <f t="shared" si="1"/>
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N9" s="5">
-        <v>710</v>
+        <v>1690</v>
       </c>
       <c r="O9" s="8">
-        <v>920</v>
+        <v>2210</v>
       </c>
       <c r="P9" s="10">
         <f t="shared" si="2"/>
-        <v>1130</v>
+        <v>2730</v>
       </c>
       <c r="Q9">
         <v>15</v>
@@ -1610,67 +1615,70 @@
         <v>11</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>128</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>130</v>
+        <v>6</v>
       </c>
       <c r="E10">
-        <v>2025</v>
+        <v>2013</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <f>cpi!$B$15/cpi!$B$5</f>
+        <v>1.3079752915774157</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10">
-        <v>6654.7500000000018</v>
-      </c>
-      <c r="I10">
-        <v>8151.0350000000008</v>
-      </c>
-      <c r="J10">
-        <v>9647.32</v>
-      </c>
-      <c r="K10">
-        <v>87.852499999999964</v>
-      </c>
-      <c r="L10">
-        <v>95.945416666666631</v>
-      </c>
-      <c r="M10">
-        <v>104.03833333333331</v>
+      <c r="H10" s="5">
+        <v>1800</v>
+      </c>
+      <c r="I10" s="8">
+        <v>2300</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="K10" s="5">
+        <v>95</v>
+      </c>
+      <c r="L10" s="8">
+        <v>120</v>
+      </c>
+      <c r="M10" s="10">
+        <f t="shared" si="1"/>
+        <v>145</v>
       </c>
       <c r="N10" s="5">
-        <v>0</v>
+        <v>710</v>
       </c>
       <c r="O10" s="8">
-        <v>0</v>
+        <v>920</v>
       </c>
       <c r="P10" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1130</v>
       </c>
       <c r="Q10">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>129</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="29" x14ac:dyDescent="0.35">
@@ -1684,7 +1692,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11">
         <v>2025</v>
@@ -1696,22 +1704,22 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>7864.9399999999987</v>
+        <v>6654.7500000000018</v>
       </c>
       <c r="I11">
-        <v>8664.32</v>
+        <v>8151.0350000000008</v>
       </c>
       <c r="J11">
-        <v>9463.6999999999989</v>
+        <v>9647.32</v>
       </c>
       <c r="K11">
-        <v>93.546666666666681</v>
+        <v>87.852499999999964</v>
       </c>
       <c r="L11">
-        <v>102.6179166666667</v>
+        <v>95.945416666666631</v>
       </c>
       <c r="M11">
-        <v>111.68916666666671</v>
+        <v>104.03833333333331</v>
       </c>
       <c r="N11" s="5">
         <v>0</v>
@@ -1738,13 +1746,13 @@
         <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
       <c r="E12">
         <v>2025</v>
@@ -1755,23 +1763,23 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8">
-        <v>0</v>
-      </c>
-      <c r="J12" s="10">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
-        <v>0</v>
-      </c>
-      <c r="L12" s="8">
-        <v>0</v>
-      </c>
-      <c r="M12" s="10">
-        <v>0</v>
+      <c r="H12">
+        <v>7864.9399999999987</v>
+      </c>
+      <c r="I12">
+        <v>8664.32</v>
+      </c>
+      <c r="J12">
+        <v>9463.6999999999989</v>
+      </c>
+      <c r="K12">
+        <v>93.546666666666681</v>
+      </c>
+      <c r="L12">
+        <v>102.6179166666667</v>
+      </c>
+      <c r="M12">
+        <v>111.68916666666671</v>
       </c>
       <c r="N12" s="5">
         <v>0</v>
@@ -1784,18 +1792,77 @@
         <v>0</v>
       </c>
       <c r="Q12">
+        <v>25</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>2025</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5">
+        <v>3700</v>
+      </c>
+      <c r="I13" s="8">
+        <v>4800</v>
+      </c>
+      <c r="J13" s="10">
+        <v>5900</v>
+      </c>
+      <c r="K13" s="5">
+        <v>42</v>
+      </c>
+      <c r="L13" s="8">
+        <v>55</v>
+      </c>
+      <c r="M13" s="10">
+        <v>68</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0</v>
+      </c>
+      <c r="P13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q13">
         <v>15</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:B9">
-    <sortCondition descending="1" ref="B7:B9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:B10">
+    <sortCondition descending="1" ref="B8:B10"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1805,11 +1872,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C73B86-AA0C-4F9D-B521-F691E24A6513}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1951,18 +2018,18 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3">
         <v>2025</v>
@@ -1974,22 +2041,22 @@
         <v>1</v>
       </c>
       <c r="H3" s="5">
-        <v>377.79000000000019</v>
+        <v>5656.3749999999991</v>
       </c>
       <c r="I3" s="8">
-        <v>438.7199999999998</v>
+        <v>6211.7216666666664</v>
       </c>
       <c r="J3" s="10">
-        <v>660.34999999999991</v>
+        <v>6767.0683333333327</v>
       </c>
       <c r="K3" s="5">
-        <v>31.482500000000016</v>
+        <v>82.112500000000054</v>
       </c>
       <c r="L3" s="8">
-        <v>36.559999999999981</v>
+        <v>91.119166666666672</v>
       </c>
       <c r="M3" s="10">
-        <v>55.029166666666661</v>
+        <v>100.1258333333333</v>
       </c>
       <c r="N3" s="5">
         <v>0</v>
@@ -2004,7 +2071,7 @@
         <v>25</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>137</v>
@@ -2015,13 +2082,13 @@
         <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>134</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="E4">
         <v>2025</v>
@@ -2033,22 +2100,22 @@
         <v>1</v>
       </c>
       <c r="H4" s="5">
-        <v>6188.8900000000021</v>
+        <v>377.79000000000019</v>
       </c>
       <c r="I4" s="8">
-        <v>11237.48</v>
+        <v>438.7199999999998</v>
       </c>
       <c r="J4" s="10">
-        <v>16286.07</v>
+        <v>660.34999999999991</v>
       </c>
       <c r="K4" s="5">
-        <v>515.74083333333351</v>
+        <v>31.482500000000016</v>
       </c>
       <c r="L4" s="8">
-        <v>936.45666666666659</v>
+        <v>36.559999999999981</v>
       </c>
       <c r="M4" s="10">
-        <v>1357.1724999999999</v>
+        <v>55.029166666666661</v>
       </c>
       <c r="N4" s="5">
         <v>0</v>
@@ -2071,16 +2138,16 @@
     </row>
     <row r="5" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>130</v>
+      <c r="D5" t="s">
+        <v>3</v>
       </c>
       <c r="E5">
         <v>2025</v>
@@ -2091,23 +2158,23 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
+      <c r="H5" s="5">
+        <v>6188.8900000000021</v>
+      </c>
+      <c r="I5" s="8">
+        <v>11237.48</v>
+      </c>
+      <c r="J5" s="10">
+        <v>16286.07</v>
+      </c>
+      <c r="K5" s="5">
+        <v>515.74083333333351</v>
+      </c>
+      <c r="L5" s="8">
+        <v>936.45666666666659</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1357.1724999999999</v>
       </c>
       <c r="N5" s="5">
         <v>0</v>
@@ -2116,17 +2183,16 @@
         <v>0</v>
       </c>
       <c r="P5" s="10">
-        <f t="shared" ref="P5:P6" si="0">$O5+($O5-$N5)</f>
         <v>0</v>
       </c>
       <c r="Q5">
         <v>25</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
@@ -2140,7 +2206,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6">
         <v>2025</v>
@@ -2176,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="P6:P7" si="0">$O6+($O6-$N6)</f>
         <v>0</v>
       </c>
       <c r="Q6">
@@ -2186,6 +2252,66 @@
         <v>132</v>
       </c>
       <c r="S6" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7">
+        <v>2025</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>25</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to use Trane Technologies costs for alternative equipment instead of NREMDB data from NREL
</commit_message>
<xml_diff>
--- a/retrofit_costs/tare_retrofit_costs_cpi.xlsx
+++ b/retrofit_costs/tare_retrofit_costs_cpi.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnav\Documents\Research\Trane_Technologies\cmu-tare-model\retrofit_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF23C1C4-9ABF-4CF4-B1B7-C133CB20563F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15FE9D0-F0AC-400F-AB87-7971826EA435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="738" firstSheet="1" activeTab="1" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="738" firstSheet="1" activeTab="2" xr2:uid="{70DC9CED-C629-4E9F-9754-D0C323F00C27}"/>
   </bookViews>
   <sheets>
     <sheet name="cpi" sheetId="7" r:id="rId1"/>
     <sheet name="heating_costs" sheetId="1" r:id="rId2"/>
     <sheet name="cooling_costs" sheetId="8" r:id="rId3"/>
-    <sheet name="waterHeating_costs" sheetId="3" r:id="rId4"/>
-    <sheet name="clothesDrying_costs" sheetId="4" r:id="rId5"/>
-    <sheet name="cooking_costs" sheetId="5" r:id="rId6"/>
-    <sheet name="enclosure_upgrade_costs" sheetId="6" r:id="rId7"/>
+    <sheet name="comparison" sheetId="9" r:id="rId4"/>
+    <sheet name="waterHeating_costs" sheetId="3" r:id="rId5"/>
+    <sheet name="clothesDrying_costs" sheetId="4" r:id="rId6"/>
+    <sheet name="cooking_costs" sheetId="5" r:id="rId7"/>
+    <sheet name="enclosure_upgrade_costs" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="148">
   <si>
     <t>$/unit</t>
   </si>
@@ -471,6 +472,21 @@
   </si>
   <si>
     <t>96 AFUE</t>
+  </si>
+  <si>
+    <t>Data Year 2013. This should NOT be zeroed out, as it was previously</t>
+  </si>
+  <si>
+    <t>Low Value</t>
+  </si>
+  <si>
+    <t>Reference Value</t>
+  </si>
+  <si>
+    <t>High Value</t>
+  </si>
+  <si>
+    <t>Generic</t>
   </si>
 </sst>
 </file>
@@ -1046,9 +1062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25BD77E-F6CE-47DE-940C-0B686D6456B3}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1479,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="10">
-        <f t="shared" ref="P7:P13" si="2">$O7+($O7-$N7)</f>
+        <f t="shared" ref="P7:P12" si="2">$O7+($O7-$N7)</f>
         <v>0</v>
       </c>
       <c r="Q7">
@@ -1857,7 +1873,7 @@
         <v>11</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>24</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1874,9 +1890,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C73B86-AA0C-4F9D-B521-F691E24A6513}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2322,6 +2338,97 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34420208-82C3-4659-A137-8BC8A5CE3502}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3">
+        <f>cooling_costs!F3*cooling_costs!G3*(cooling_costs!H3+2*12*cooling_costs!K3)</f>
+        <v>7627.0750000000007</v>
+      </c>
+      <c r="C3">
+        <f>cooling_costs!F2*cooling_costs!G2*(cooling_costs!H2+2*12*cooling_costs!K2)</f>
+        <v>8186.91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <f>heating_costs!F3*heating_costs!G3*(heating_costs!H3+2*12*heating_costs!K3)</f>
+        <v>3481.0560000000005</v>
+      </c>
+      <c r="C4">
+        <f>heating_costs!F2*heating_costs!G2*(heating_costs!H2+2*12*heating_costs!K2)</f>
+        <v>3392.3647162351849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <f>heating_costs!F11*heating_costs!G11*(heating_costs!H11+2*12*heating_costs!K11)</f>
+        <v>8763.2100000000009</v>
+      </c>
+      <c r="C5">
+        <f>heating_costs!F7*heating_costs!G7*(heating_costs!H7+2*12*heating_costs!K7)</f>
+        <v>6157.9476727464726</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FBB1F9-AA0F-4F3E-92E1-FA5D825DBAEF}">
   <dimension ref="A1:T95"/>
   <sheetViews>
@@ -3607,7 +3714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51DF997B-B96C-4908-A8E2-238F90744569}">
   <dimension ref="A1:N101"/>
   <sheetViews>
@@ -4379,7 +4486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4F662D-1BD7-4400-95A3-A4A7CEFF8447}">
   <dimension ref="A1:N102"/>
   <sheetViews>
@@ -5077,7 +5184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AAB083-F7AB-4F7C-A5E9-54BE3CB88F43}">
   <dimension ref="A1:L24"/>
   <sheetViews>

</xml_diff>